<commit_message>
Many many changes, IDK
</commit_message>
<xml_diff>
--- a/4° Año/2° Semestre/Investigacion operativa/2 PROGRAMACIÓN LINEAL - PRÁCTICA/TP1 parte B.xlsx
+++ b/4° Año/2° Semestre/Investigacion operativa/2 PROGRAMACIÓN LINEAL - PRÁCTICA/TP1 parte B.xlsx
@@ -1,21 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Lucas\Documents\facultad\4° Año\2° Semestre\Investigacion operativa\2 PROGRAMACIÓN LINEAL - PRÁCTICA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B2AEF6B-788E-4B67-9C64-D234D9B9D7E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C63D90A-3E97-4486-BE43-4D6E5F8620C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{E7CE275C-18B3-4C2F-911A-6C3807A7ABB6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{E7CE275C-18B3-4C2F-911A-6C3807A7ABB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Parte A - Ej 4" sheetId="1" r:id="rId1"/>
     <sheet name="Ej 5" sheetId="2" r:id="rId2"/>
     <sheet name="Ej 7" sheetId="3" r:id="rId3"/>
+    <sheet name="Ej 8" sheetId="4" r:id="rId4"/>
+    <sheet name="Ej 9" sheetId="5" r:id="rId5"/>
+    <sheet name="Ej 10" sheetId="6" r:id="rId6"/>
+    <sheet name="Ej 11" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="20">
   <si>
     <t>Tabla1</t>
   </si>
@@ -85,12 +89,15 @@
   <si>
     <t>El maximo Z es 19800 y se obtiene fabricando 120 celeron y 300 pentium</t>
   </si>
+  <si>
+    <t>S0</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,6 +110,12 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -158,7 +171,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -181,14 +194,26 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -538,7 +563,7 @@
       <c r="H3" s="3">
         <v>0</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="12" t="s">
         <v>11</v>
       </c>
     </row>
@@ -567,7 +592,7 @@
       <c r="H4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="9"/>
+      <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -660,10 +685,10 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="4">
         <f>SUMPRODUCT($B$5:$B$7,C5:C7)</f>
         <v>0</v>
@@ -690,11 +715,11 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
       <c r="D9" s="4">
         <f>D3-D8</f>
         <v>12</v>
@@ -739,7 +764,7 @@
       <c r="H12" s="3">
         <v>0</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="12" t="s">
         <v>11</v>
       </c>
     </row>
@@ -768,7 +793,7 @@
       <c r="H13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I13" s="9"/>
+      <c r="I13" s="13"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -786,7 +811,7 @@
         <v>0</v>
       </c>
       <c r="E14" s="7">
-        <f t="shared" ref="D14:H14" si="3">E5-($D$5*E15)</f>
+        <f t="shared" ref="E14:H14" si="3">E5-($D$5*E15)</f>
         <v>0.28000000000000003</v>
       </c>
       <c r="F14" s="2">
@@ -879,10 +904,10 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="5"/>
+      <c r="B17" s="14"/>
       <c r="C17" s="4">
         <f>SUMPRODUCT($B14:$B16,C14:C16)</f>
         <v>2880</v>
@@ -909,11 +934,11 @@
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
       <c r="D18" s="3">
         <f>D12-D17</f>
         <v>0</v>
@@ -958,7 +983,7 @@
       <c r="H21" s="3">
         <v>0</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="I21" s="12" t="s">
         <v>11</v>
       </c>
     </row>
@@ -987,7 +1012,7 @@
       <c r="H22" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I22" s="9"/>
+      <c r="I22" s="13"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
@@ -1034,7 +1059,7 @@
         <v>200</v>
       </c>
       <c r="D24" s="2">
-        <f t="shared" ref="D24:I24" si="13">D15-($E15*D23)</f>
+        <f t="shared" ref="D24:H24" si="13">D15-($E15*D23)</f>
         <v>1</v>
       </c>
       <c r="E24" s="2">
@@ -1089,10 +1114,10 @@
       <c r="I25" s="2"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="5"/>
+      <c r="B26" s="14"/>
       <c r="C26" s="4">
         <f>SUMPRODUCT($B23:$B25,C23:C25)</f>
         <v>3300</v>
@@ -1119,11 +1144,11 @@
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
       <c r="D27" s="3">
         <f>D21-D26</f>
         <v>0</v>
@@ -1146,13 +1171,12 @@
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A29" s="10" t="s">
+      <c r="A29" s="9" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="I21:I22"/>
     <mergeCell ref="A26:B26"/>
     <mergeCell ref="A27:C27"/>
     <mergeCell ref="A8:B8"/>
@@ -1161,6 +1185,7 @@
     <mergeCell ref="I12:I13"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A18:C18"/>
+    <mergeCell ref="I21:I22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1200,7 +1225,7 @@
       <c r="H3" s="3">
         <v>0</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="12" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1229,7 +1254,7 @@
       <c r="H4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="9"/>
+      <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -1322,10 +1347,10 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="4">
         <f>SUMPRODUCT($B5:$B7,C5:C7)</f>
         <v>0</v>
@@ -1353,11 +1378,11 @@
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
       <c r="D9" s="3">
         <f>D3-D8</f>
         <v>40</v>
@@ -1403,7 +1428,7 @@
       <c r="H12" s="3">
         <v>0</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="12" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1432,7 +1457,7 @@
       <c r="H13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I13" s="9"/>
+      <c r="I13" s="13"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -1543,10 +1568,10 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="5"/>
+      <c r="B17" s="14"/>
       <c r="C17" s="4">
         <f>SUMPRODUCT($B14:$B16,C14:C16)</f>
         <v>18000</v>
@@ -1574,11 +1599,11 @@
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
       <c r="D18" s="4">
         <f>D12-D17</f>
         <v>15</v>
@@ -1624,7 +1649,7 @@
       <c r="H21" s="3">
         <v>0</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="I21" s="12" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1653,7 +1678,7 @@
       <c r="H22" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I22" s="9"/>
+      <c r="I22" s="13"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
@@ -1755,10 +1780,10 @@
       <c r="I25" s="2"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="5"/>
+      <c r="B26" s="14"/>
       <c r="C26" s="4">
         <f>SUMPRODUCT($B23:$B25,C23:C25)</f>
         <v>19800</v>
@@ -1786,11 +1811,11 @@
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
       <c r="D27" s="3">
         <f>D21-D26</f>
         <v>0</v>
@@ -1838,8 +1863,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07A0899-685B-4FDE-A77E-817489045368}">
   <dimension ref="A3:I30"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1867,7 +1892,7 @@
       <c r="H3" s="3">
         <v>0</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="I3" s="12" t="s">
         <v>11</v>
       </c>
     </row>
@@ -1896,7 +1921,7 @@
       <c r="H4" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I4" s="9"/>
+      <c r="I4" s="13"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
@@ -1989,10 +2014,10 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="5" t="s">
+      <c r="A8" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="5"/>
+      <c r="B8" s="14"/>
       <c r="C8" s="4">
         <f>SUMPRODUCT($B$5:$B$7,C5:C7)</f>
         <v>0</v>
@@ -2020,11 +2045,11 @@
       <c r="I8" s="1"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="5" t="s">
+      <c r="A9" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="5"/>
-      <c r="C9" s="5"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
       <c r="D9" s="4">
         <f>D3-D8</f>
         <v>4</v>
@@ -2070,7 +2095,7 @@
       <c r="H12" s="3">
         <v>0</v>
       </c>
-      <c r="I12" s="8" t="s">
+      <c r="I12" s="12" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2099,7 +2124,7 @@
       <c r="H13" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I13" s="9"/>
+      <c r="I13" s="13"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
@@ -2210,10 +2235,10 @@
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B17" s="5"/>
+      <c r="B17" s="14"/>
       <c r="C17" s="4">
         <f>SUMPRODUCT($B14:$B16,C14:C16)</f>
         <v>14000</v>
@@ -2241,11 +2266,11 @@
       <c r="I17" s="1"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+      <c r="B18" s="14"/>
+      <c r="C18" s="14"/>
       <c r="D18" s="3">
         <f>D12-D17</f>
         <v>0</v>
@@ -2291,7 +2316,7 @@
       <c r="H21" s="3">
         <v>0</v>
       </c>
-      <c r="I21" s="8" t="s">
+      <c r="I21" s="12" t="s">
         <v>11</v>
       </c>
     </row>
@@ -2320,7 +2345,7 @@
       <c r="H22" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="I22" s="9"/>
+      <c r="I22" s="13"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
@@ -2422,10 +2447,10 @@
       <c r="I25" s="2"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
+      <c r="A26" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="5"/>
+      <c r="B26" s="14"/>
       <c r="C26" s="4">
         <f>SUMPRODUCT($B23:$B25,C23:C25)</f>
         <v>15000</v>
@@ -2453,11 +2478,11 @@
       <c r="I26" s="1"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B27" s="5"/>
-      <c r="C27" s="5"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="14"/>
       <c r="D27" s="3">
         <f>D21-D26</f>
         <v>0</v>
@@ -2499,4 +2524,1292 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E768D8-EA0F-4F11-8D5F-973E50DB4C7E}">
+  <dimension ref="A3:J20"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5">
+        <f>105.41*10</f>
+        <v>1054.0999999999999</v>
+      </c>
+      <c r="E3" s="5">
+        <f>119.6*6</f>
+        <v>717.59999999999991</v>
+      </c>
+      <c r="F3" s="11">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="5">
+        <v>0</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="13"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="10">
+        <v>0</v>
+      </c>
+      <c r="C5" s="10">
+        <v>70</v>
+      </c>
+      <c r="D5" s="10">
+        <v>1</v>
+      </c>
+      <c r="E5" s="10">
+        <v>1</v>
+      </c>
+      <c r="F5" s="10">
+        <v>1</v>
+      </c>
+      <c r="G5" s="10">
+        <v>0</v>
+      </c>
+      <c r="H5" s="10">
+        <v>0</v>
+      </c>
+      <c r="I5" s="10">
+        <v>0</v>
+      </c>
+      <c r="J5" s="10">
+        <f>C5/D5</f>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="8">
+        <v>0</v>
+      </c>
+      <c r="C6" s="8">
+        <v>7500</v>
+      </c>
+      <c r="D6" s="8">
+        <v>110</v>
+      </c>
+      <c r="E6" s="10">
+        <v>95</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8">
+        <v>1</v>
+      </c>
+      <c r="H6" s="8">
+        <v>0</v>
+      </c>
+      <c r="I6" s="8">
+        <v>0</v>
+      </c>
+      <c r="J6" s="10">
+        <f t="shared" ref="J6:J8" si="0">C6/D6</f>
+        <v>68.181818181818187</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="8">
+        <v>0</v>
+      </c>
+      <c r="C7" s="8">
+        <v>57900</v>
+      </c>
+      <c r="D7" s="7">
+        <v>900</v>
+      </c>
+      <c r="E7" s="8">
+        <v>650</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1</v>
+      </c>
+      <c r="I7" s="8">
+        <v>0</v>
+      </c>
+      <c r="J7" s="10">
+        <f t="shared" si="0"/>
+        <v>64.333333333333329</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="8">
+        <v>0</v>
+      </c>
+      <c r="C8" s="8">
+        <v>115200</v>
+      </c>
+      <c r="D8" s="8">
+        <v>1200</v>
+      </c>
+      <c r="E8" s="8">
+        <v>850</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0</v>
+      </c>
+      <c r="G8" s="8">
+        <v>0</v>
+      </c>
+      <c r="H8" s="8">
+        <v>0</v>
+      </c>
+      <c r="I8" s="8">
+        <v>1</v>
+      </c>
+      <c r="J8" s="10">
+        <f t="shared" si="0"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="4">
+        <f>SUMPRODUCT($B5:$B8,C5:C8)</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="11">
+        <f t="shared" ref="D9:I9" si="1">SUMPRODUCT($B5:$B8,D5:D8)</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="4">
+        <f>D3-D9</f>
+        <v>1054.0999999999999</v>
+      </c>
+      <c r="E10" s="11">
+        <f t="shared" ref="E10:I10" si="2">E3-E9</f>
+        <v>717.59999999999991</v>
+      </c>
+      <c r="F10" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="1"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="6"/>
+      <c r="C13" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D13" s="11">
+        <f>105.41*10</f>
+        <v>1054.0999999999999</v>
+      </c>
+      <c r="E13" s="11">
+        <f>119.6*6</f>
+        <v>717.59999999999991</v>
+      </c>
+      <c r="F13" s="11">
+        <v>0</v>
+      </c>
+      <c r="G13" s="11">
+        <v>0</v>
+      </c>
+      <c r="H13" s="11">
+        <v>0</v>
+      </c>
+      <c r="I13" s="11">
+        <v>0</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J14" s="13"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="10">
+        <v>0</v>
+      </c>
+      <c r="C15" s="10">
+        <f>C5-(C17*$D$5)</f>
+        <v>5.6666666666666714</v>
+      </c>
+      <c r="D15" s="10">
+        <f t="shared" ref="D15:I15" si="3">D5-(D17*$D$5)</f>
+        <v>0</v>
+      </c>
+      <c r="E15" s="10">
+        <f t="shared" si="3"/>
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="F15" s="10">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="G15" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="H15" s="10">
+        <f t="shared" si="3"/>
+        <v>-1.1111111111111111E-3</v>
+      </c>
+      <c r="I15" s="10">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="J15" s="10"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" s="10">
+        <v>0</v>
+      </c>
+      <c r="C16" s="10">
+        <f>C6-(C17*$D$6)</f>
+        <v>423.33333333333394</v>
+      </c>
+      <c r="D16" s="10">
+        <f t="shared" ref="D16:I16" si="4">D6-(D17*$D$6)</f>
+        <v>0</v>
+      </c>
+      <c r="E16" s="10">
+        <f t="shared" si="4"/>
+        <v>15.555555555555557</v>
+      </c>
+      <c r="F16" s="10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="G16" s="10">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+      <c r="H16" s="10">
+        <f t="shared" si="4"/>
+        <v>-0.12222222222222222</v>
+      </c>
+      <c r="I16" s="10">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="J16" s="10"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="10">
+        <f>105.41*10</f>
+        <v>1054.0999999999999</v>
+      </c>
+      <c r="C17" s="10">
+        <f>C7/$D$7</f>
+        <v>64.333333333333329</v>
+      </c>
+      <c r="D17" s="10">
+        <f t="shared" ref="D17:I17" si="5">D7/$D$7</f>
+        <v>1</v>
+      </c>
+      <c r="E17" s="10">
+        <f t="shared" si="5"/>
+        <v>0.72222222222222221</v>
+      </c>
+      <c r="F17" s="10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="G17" s="10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="H17" s="10">
+        <f t="shared" si="5"/>
+        <v>1.1111111111111111E-3</v>
+      </c>
+      <c r="I17" s="10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="J17" s="10"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="10">
+        <v>0</v>
+      </c>
+      <c r="C18" s="10">
+        <f>C8-(C17*$D$8)</f>
+        <v>38000</v>
+      </c>
+      <c r="D18" s="10">
+        <f t="shared" ref="D18:I18" si="6">D8-(D17*$D$8)</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="10">
+        <f t="shared" si="6"/>
+        <v>-16.666666666666629</v>
+      </c>
+      <c r="F18" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G18" s="10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="H18" s="10">
+        <f t="shared" si="6"/>
+        <v>-1.3333333333333333</v>
+      </c>
+      <c r="I18" s="10">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="J18" s="10"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="14"/>
+      <c r="C19" s="4">
+        <f>SUMPRODUCT($B15:$B18,C15:C18)</f>
+        <v>67813.766666666663</v>
+      </c>
+      <c r="D19" s="11">
+        <f>SUMPRODUCT($B15:$B18,D15:D18)</f>
+        <v>1054.0999999999999</v>
+      </c>
+      <c r="E19" s="11">
+        <f>SUMPRODUCT($B15:$B18,E15:E18)</f>
+        <v>761.29444444444437</v>
+      </c>
+      <c r="F19" s="11">
+        <f>SUMPRODUCT($B15:$B18,F15:F18)</f>
+        <v>0</v>
+      </c>
+      <c r="G19" s="11">
+        <f>SUMPRODUCT($B15:$B18,G15:G18)</f>
+        <v>0</v>
+      </c>
+      <c r="H19" s="11">
+        <f>SUMPRODUCT($B15:$B18,H15:H18)</f>
+        <v>1.1712222222222222</v>
+      </c>
+      <c r="I19" s="11">
+        <f>SUMPRODUCT($B15:$B18,I15:I18)</f>
+        <v>0</v>
+      </c>
+      <c r="J19" s="1"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="14"/>
+      <c r="C20" s="14"/>
+      <c r="D20" s="11">
+        <f>D13-D19</f>
+        <v>0</v>
+      </c>
+      <c r="E20" s="11">
+        <f t="shared" ref="E20:I20" si="7">E13-E19</f>
+        <v>-43.694444444444457</v>
+      </c>
+      <c r="F20" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="G20" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H20" s="11">
+        <f t="shared" si="7"/>
+        <v>-1.1712222222222222</v>
+      </c>
+      <c r="I20" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="J20" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="A20:C20"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="J13:J14"/>
+  </mergeCells>
+  <phoneticPr fontId="2" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0909A2B5-D8DD-4C1F-B173-AAD6115DCC82}">
+  <dimension ref="A3:J10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="11">
+        <v>24</v>
+      </c>
+      <c r="E3" s="11">
+        <v>16</v>
+      </c>
+      <c r="F3" s="11">
+        <v>0</v>
+      </c>
+      <c r="G3" s="11">
+        <v>0</v>
+      </c>
+      <c r="H3" s="11">
+        <v>0</v>
+      </c>
+      <c r="I3" s="11">
+        <v>0</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J4" s="13"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="10">
+        <v>0</v>
+      </c>
+      <c r="C5" s="10">
+        <v>12</v>
+      </c>
+      <c r="D5" s="10">
+        <v>1</v>
+      </c>
+      <c r="E5" s="10">
+        <v>1</v>
+      </c>
+      <c r="F5" s="10">
+        <v>1</v>
+      </c>
+      <c r="G5" s="10">
+        <v>0</v>
+      </c>
+      <c r="H5" s="10">
+        <v>0</v>
+      </c>
+      <c r="I5" s="10">
+        <v>0</v>
+      </c>
+      <c r="J5" s="10">
+        <f>C5/D5</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="10">
+        <v>0</v>
+      </c>
+      <c r="C6" s="10">
+        <v>11</v>
+      </c>
+      <c r="D6" s="10">
+        <v>1</v>
+      </c>
+      <c r="E6" s="10">
+        <v>0</v>
+      </c>
+      <c r="F6" s="10">
+        <v>0</v>
+      </c>
+      <c r="G6" s="10">
+        <v>1</v>
+      </c>
+      <c r="H6" s="10">
+        <v>0</v>
+      </c>
+      <c r="I6" s="10">
+        <v>0</v>
+      </c>
+      <c r="J6" s="10">
+        <f t="shared" ref="J6:J8" si="0">C6/D6</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="10">
+        <v>0</v>
+      </c>
+      <c r="C7" s="10">
+        <v>22</v>
+      </c>
+      <c r="D7" s="7">
+        <v>1</v>
+      </c>
+      <c r="E7" s="10">
+        <v>1</v>
+      </c>
+      <c r="F7" s="10">
+        <v>0</v>
+      </c>
+      <c r="G7" s="10">
+        <v>0</v>
+      </c>
+      <c r="H7" s="10">
+        <v>1</v>
+      </c>
+      <c r="I7" s="10">
+        <v>0</v>
+      </c>
+      <c r="J7" s="10">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="10">
+        <v>0</v>
+      </c>
+      <c r="C8" s="10">
+        <v>400</v>
+      </c>
+      <c r="D8" s="10">
+        <v>40</v>
+      </c>
+      <c r="E8" s="10">
+        <v>20</v>
+      </c>
+      <c r="F8" s="10">
+        <v>0</v>
+      </c>
+      <c r="G8" s="10">
+        <v>0</v>
+      </c>
+      <c r="H8" s="10">
+        <v>0</v>
+      </c>
+      <c r="I8" s="10">
+        <v>1</v>
+      </c>
+      <c r="J8" s="10">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="4">
+        <f>SUMPRODUCT($B5:$B8,C5:C8)</f>
+        <v>0</v>
+      </c>
+      <c r="D9" s="11">
+        <f t="shared" ref="D9:I9" si="1">SUMPRODUCT($B5:$B8,D5:D8)</f>
+        <v>0</v>
+      </c>
+      <c r="E9" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="4">
+        <f>D3-D9</f>
+        <v>24</v>
+      </c>
+      <c r="E10" s="11">
+        <f t="shared" ref="E10:I10" si="2">E3-E9</f>
+        <v>16</v>
+      </c>
+      <c r="F10" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J10" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="J3:J4"/>
+    <mergeCell ref="A9:B9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCC383D6-9DC4-4FA9-8E30-184B5974B15D}">
+  <dimension ref="A3:I9"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:I9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5">
+        <v>4</v>
+      </c>
+      <c r="E3" s="5">
+        <v>3</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="13"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="8">
+        <v>0</v>
+      </c>
+      <c r="C5" s="8">
+        <v>48000</v>
+      </c>
+      <c r="D5" s="8">
+        <v>3</v>
+      </c>
+      <c r="E5" s="8">
+        <v>8</v>
+      </c>
+      <c r="F5" s="8">
+        <v>1</v>
+      </c>
+      <c r="G5" s="8">
+        <v>0</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0</v>
+      </c>
+      <c r="I5" s="8">
+        <f>C5/D5</f>
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="8">
+        <v>0</v>
+      </c>
+      <c r="C6" s="8">
+        <v>42000</v>
+      </c>
+      <c r="D6" s="7">
+        <v>12</v>
+      </c>
+      <c r="E6" s="8">
+        <v>6</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8">
+        <v>1</v>
+      </c>
+      <c r="H6" s="8">
+        <v>0</v>
+      </c>
+      <c r="I6" s="8">
+        <f t="shared" ref="I6:I7" si="0">C6/D6</f>
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="8">
+        <v>0</v>
+      </c>
+      <c r="C7" s="8">
+        <v>36000</v>
+      </c>
+      <c r="D7" s="8">
+        <v>9</v>
+      </c>
+      <c r="E7" s="8">
+        <v>9</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1</v>
+      </c>
+      <c r="I7" s="8">
+        <f t="shared" si="0"/>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="4">
+        <f>SUMPRODUCT($B$5:$B$7,C5:C7)</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <f>SUMPRODUCT($B$5:$B$7,D5:D7)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="5">
+        <f>SUMPRODUCT($B$5:$B$7,E5:E7)</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
+        <f t="shared" ref="F8:H8" si="1">SUMPRODUCT($B$5:$B$7,F5:F7)</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="4">
+        <f>D3-D8</f>
+        <v>4</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" ref="E9:H9" si="2">E3-E8</f>
+        <v>3</v>
+      </c>
+      <c r="F9" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:C9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F485CE0-8B47-41FB-BCFC-81CEA9BA3E4B}">
+  <dimension ref="A3:I9"/>
+  <sheetViews>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" s="6"/>
+      <c r="C3" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="5">
+        <v>4</v>
+      </c>
+      <c r="E3" s="5">
+        <v>3</v>
+      </c>
+      <c r="F3" s="5">
+        <v>0</v>
+      </c>
+      <c r="G3" s="5">
+        <v>0</v>
+      </c>
+      <c r="H3" s="5">
+        <v>0</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="13"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="8">
+        <v>0</v>
+      </c>
+      <c r="C5" s="8">
+        <v>48000</v>
+      </c>
+      <c r="D5" s="8">
+        <v>3</v>
+      </c>
+      <c r="E5" s="8">
+        <v>8</v>
+      </c>
+      <c r="F5" s="8">
+        <v>1</v>
+      </c>
+      <c r="G5" s="8">
+        <v>0</v>
+      </c>
+      <c r="H5" s="8">
+        <v>0</v>
+      </c>
+      <c r="I5" s="8">
+        <f>C5/D5</f>
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="8">
+        <v>0</v>
+      </c>
+      <c r="C6" s="8">
+        <v>42000</v>
+      </c>
+      <c r="D6" s="7">
+        <v>12</v>
+      </c>
+      <c r="E6" s="8">
+        <v>6</v>
+      </c>
+      <c r="F6" s="8">
+        <v>0</v>
+      </c>
+      <c r="G6" s="8">
+        <v>1</v>
+      </c>
+      <c r="H6" s="8">
+        <v>0</v>
+      </c>
+      <c r="I6" s="8">
+        <f t="shared" ref="I6:I7" si="0">C6/D6</f>
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="8">
+        <v>0</v>
+      </c>
+      <c r="C7" s="8">
+        <v>36000</v>
+      </c>
+      <c r="D7" s="8">
+        <v>9</v>
+      </c>
+      <c r="E7" s="8">
+        <v>9</v>
+      </c>
+      <c r="F7" s="8">
+        <v>0</v>
+      </c>
+      <c r="G7" s="8">
+        <v>0</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1</v>
+      </c>
+      <c r="I7" s="8">
+        <f t="shared" si="0"/>
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="14" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="14"/>
+      <c r="C8" s="4">
+        <f>SUMPRODUCT($B$5:$B$7,C5:C7)</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="5">
+        <f>SUMPRODUCT($B$5:$B$7,D5:D7)</f>
+        <v>0</v>
+      </c>
+      <c r="E8" s="5">
+        <f>SUMPRODUCT($B$5:$B$7,E5:E7)</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="5">
+        <f t="shared" ref="F8:H8" si="1">SUMPRODUCT($B$5:$B$7,F5:F7)</f>
+        <v>0</v>
+      </c>
+      <c r="G8" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H8" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="I8" s="1"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="4">
+        <f>D3-D8</f>
+        <v>4</v>
+      </c>
+      <c r="E9" s="5">
+        <f t="shared" ref="E9:H9" si="2">E3-E8</f>
+        <v>3</v>
+      </c>
+      <c r="F9" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="I3:I4"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:C9"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
antes de cambiar ubuntu
</commit_message>
<xml_diff>
--- a/4° Año/2° Semestre/Investigacion operativa/2 PROGRAMACIÓN LINEAL - PRÁCTICA/TP1 parte B.xlsx
+++ b/4° Año/2° Semestre/Investigacion operativa/2 PROGRAMACIÓN LINEAL - PRÁCTICA/TP1 parte B.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Lucas\Documents\facultad\4° Año\2° Semestre\Investigacion operativa\2 PROGRAMACIÓN LINEAL - PRÁCTICA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9EFF2BC-2E15-4AC6-BC34-0698C3DDD943}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D669CA6-A4D3-43D6-99DD-63020565E65E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="6" xr2:uid="{E7CE275C-18B3-4C2F-911A-6C3807A7ABB6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{E7CE275C-18B3-4C2F-911A-6C3807A7ABB6}"/>
   </bookViews>
   <sheets>
     <sheet name="Parte A - Ej 4 y Parte B - Ej 6" sheetId="1" r:id="rId1"/>
@@ -21,17 +21,27 @@
     <sheet name="Ej 10" sheetId="6" r:id="rId6"/>
     <sheet name="Ej 11" sheetId="7" r:id="rId7"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Ej 8'!$A$1:$J$32</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="857" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="847" uniqueCount="54">
   <si>
     <t>Tabla1</t>
   </si>
@@ -93,9 +103,6 @@
     <t>A3</t>
   </si>
   <si>
-    <t>Nota5: Si tita da &lt; 0 ignorar (no seleccionar como pivote)</t>
-  </si>
-  <si>
     <t>Solucion optima: Z=256, X1=8, X2=4</t>
   </si>
   <si>
@@ -118,24 +125,6 @@
   </si>
   <si>
     <t>Solucion: Z=76, X1=4, X2=9</t>
-  </si>
-  <si>
-    <t>Nota1: Con resticciones &gt;= poner una variable de holgura (-) y una artificial (+)</t>
-  </si>
-  <si>
-    <t>Nota2: Para minimizar todas las variables de Z se las multiplicar por -1</t>
-  </si>
-  <si>
-    <t>Nota3: Buscar para la columna pivote el mayor numero de Cj - Zj (igual)</t>
-  </si>
-  <si>
-    <t>Nota4: El criterio de tita es menor positivo (igual)</t>
-  </si>
-  <si>
-    <t>Nota6: Cuando Z se hace todo 0 (sacas las variables artificiales), reemplazar con los valores negativos de las variables en la formula Z (en la columna C) y seguir resolviendo sin las A si se puede. Osea, repetis proceso hasta sacar toda variable artificial y resolves una max</t>
-  </si>
-  <si>
-    <t>Nota7: Las variables basicas son las que Cj-Zj da 0 en la ultima tabla</t>
   </si>
   <si>
     <t>s1</t>
@@ -187,15 +176,6 @@
   </si>
   <si>
     <t>A4</t>
-  </si>
-  <si>
-    <t>Nota8: Cambiar el signo de las Cj de aquellas que antes eran &gt;=</t>
-  </si>
-  <si>
-    <t>Nota9: A las que antes era &gt;= en la matriz no se ponen con 1 sino -1 y los numeros de la matriz ya no se multiplican por -1</t>
-  </si>
-  <si>
-    <t>Nota10: Basicamente, si es &gt;= cambiar el signo de todo menos Ck</t>
   </si>
   <si>
     <t>X3</t>
@@ -759,9 +739,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4386E0A1-8924-4EBD-8F4A-62A8893B04FA}">
   <dimension ref="A3:I40"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E30" sqref="E30"/>
-    </sheetView>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1400,19 +1378,19 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D28" s="1" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="H28" s="1" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -1422,7 +1400,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B34" s="6"/>
       <c r="C34" s="14" t="s">
@@ -1458,13 +1436,13 @@
         <v>4</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="G35" s="4" t="s">
         <v>6</v>
@@ -1476,7 +1454,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B36" s="15">
         <v>100</v>
@@ -1506,7 +1484,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B37" s="15">
         <v>120</v>
@@ -1593,13 +1571,13 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D40" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F40" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G40" s="1" t="s">
         <v>13</v>
@@ -1625,6 +1603,9 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;18Ejercicio 4 y 6</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -1632,8 +1613,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DF2640C-777F-4D5C-9A94-B528B7856413}">
   <dimension ref="A3:I39"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2281,7 +2262,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="14" t="s">
@@ -2317,13 +2298,13 @@
         <v>4</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>6</v>
@@ -2335,7 +2316,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B35" s="15">
         <v>720</v>
@@ -2365,7 +2346,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B36" s="15">
         <v>1800</v>
@@ -2455,13 +2436,13 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D39" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>13</v>
@@ -2486,6 +2467,10 @@
     <mergeCell ref="A17:B17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;18Ejercicio 5</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -2493,9 +2478,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D07A0899-685B-4FDE-A77E-817489045368}">
   <dimension ref="A3:I39"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F41" sqref="F41"/>
-    </sheetView>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -3142,7 +3125,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="14" t="s">
@@ -3178,13 +3161,13 @@
         <v>4</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="F34" s="4" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="G34" s="4" t="s">
         <v>7</v>
@@ -3196,7 +3179,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="B35" s="15">
         <v>42000</v>
@@ -3227,7 +3210,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B36" s="15">
         <v>36000</v>
@@ -3317,13 +3300,13 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D39" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="G39" s="1" t="s">
         <v>13</v>
@@ -3349,6 +3332,10 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;18Ejercicio 7</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -3356,8 +3343,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C2E768D8-EA0F-4F11-8D5F-973E50DB4C7E}">
   <dimension ref="A3:J31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3420,7 +3407,7 @@
         <v>8</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="J4" s="20"/>
     </row>
@@ -3525,7 +3512,7 @@
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B8" s="8">
         <v>0</v>
@@ -3681,7 +3668,7 @@
         <v>8</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="J14" s="20"/>
     </row>
@@ -3799,7 +3786,7 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B18" s="10">
         <v>0</v>
@@ -3903,12 +3890,12 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="H21" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -3952,16 +3939,16 @@
         <v>4</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E27" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G27" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G27" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="H27" s="4" t="s">
         <v>6</v>
@@ -3973,7 +3960,7 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B28" s="15">
         <v>57900</v>
@@ -4075,16 +4062,16 @@
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D31" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="E31" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F31" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="G31" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="H31" t="s">
         <v>13</v>
@@ -4107,20 +4094,22 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="95" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;18Ejercicio 8</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0909A2B5-D8DD-4C1F-B173-AAD6115DCC82}">
-  <dimension ref="A3:N52"/>
+  <dimension ref="A3:L52"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
-    </sheetView>
+    <sheetView view="pageLayout" zoomScaleNormal="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
@@ -4155,11 +4144,8 @@
       <c r="L3" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="N3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -4185,22 +4171,19 @@
         <v>8</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="L4" s="20"/>
-      <c r="N4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="10">
         <v>-1</v>
@@ -4236,11 +4219,8 @@
         <f>C5/D5</f>
         <v>12</v>
       </c>
-      <c r="N5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
         <v>7</v>
       </c>
@@ -4278,11 +4258,8 @@
         <f>C6/D6</f>
         <v>11</v>
       </c>
-      <c r="N6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
         <v>8</v>
       </c>
@@ -4320,13 +4297,10 @@
         <f>C7/D7</f>
         <v>22</v>
       </c>
-      <c r="N7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B8" s="10">
         <v>-1</v>
@@ -4362,11 +4336,8 @@
         <f>C8/D8</f>
         <v>10</v>
       </c>
-      <c r="N8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="18" t="s">
         <v>9</v>
       </c>
@@ -4408,11 +4379,8 @@
         <v>-1</v>
       </c>
       <c r="L9" s="1"/>
-      <c r="N9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>10</v>
       </c>
@@ -4452,7 +4420,7 @@
       </c>
       <c r="L10" s="1"/>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>12</v>
       </c>
@@ -4488,7 +4456,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>2</v>
       </c>
@@ -4514,19 +4482,19 @@
         <v>8</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="L14" s="20"/>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="12">
         <v>-1</v>
@@ -4572,7 +4540,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>7</v>
       </c>
@@ -4861,13 +4829,13 @@
         <v>8</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="J24" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="K24" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="L24" s="20"/>
     </row>
@@ -5134,7 +5102,7 @@
       </c>
       <c r="L30" s="1"/>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>16</v>
       </c>
@@ -5166,7 +5134,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
         <v>2</v>
       </c>
@@ -5192,13 +5160,13 @@
         <v>8</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="J34" s="4"/>
       <c r="K34" s="4"/>
       <c r="L34" s="22"/>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="12" t="s">
         <v>14</v>
       </c>
@@ -5230,7 +5198,7 @@
       <c r="K35" s="12"/>
       <c r="L35" s="12"/>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
         <v>7</v>
       </c>
@@ -5262,7 +5230,7 @@
       <c r="K36" s="12"/>
       <c r="L36" s="12"/>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
         <v>8</v>
       </c>
@@ -5294,7 +5262,7 @@
       <c r="K37" s="12"/>
       <c r="L37" s="12"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38" s="12" t="s">
         <v>13</v>
       </c>
@@ -5326,7 +5294,7 @@
       <c r="K38" s="12"/>
       <c r="L38" s="12"/>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="23" t="s">
         <v>9</v>
       </c>
@@ -5363,7 +5331,7 @@
       <c r="K39" s="13"/>
       <c r="L39" s="1"/>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40" s="23" t="s">
         <v>10</v>
       </c>
@@ -5397,22 +5365,22 @@
       <c r="K40" s="13"/>
       <c r="L40" s="1"/>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="F41" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I41" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46" s="6" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B46" s="6"/>
       <c r="C46" s="14" t="s">
@@ -5439,11 +5407,8 @@
       <c r="J46" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="N46" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47" s="4" t="s">
         <v>2</v>
       </c>
@@ -5454,16 +5419,16 @@
         <v>4</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E47" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G47" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="H47" s="4" t="s">
         <v>6</v>
@@ -5472,13 +5437,10 @@
         <v>7</v>
       </c>
       <c r="J47" s="22"/>
-      <c r="N47" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48" s="15" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B48" s="15">
         <v>12</v>
@@ -5509,13 +5471,10 @@
         <v>-2</v>
       </c>
       <c r="J48" s="15"/>
-      <c r="N48" t="s">
-        <v>54</v>
-      </c>
     </row>
     <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49" s="15" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B49" s="15">
         <v>400</v>
@@ -5616,16 +5575,16 @@
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D52" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="H52" s="1" t="s">
         <v>13</v>
@@ -5654,6 +5613,10 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="75" orientation="portrait" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;18Ejercicio 9</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -5661,8 +5624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCC383D6-9DC4-4FA9-8E30-184B5974B15D}">
   <dimension ref="A3:Q132"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R70" sqref="R70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5735,7 +5698,7 @@
         <v>14</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>6</v>
@@ -5747,25 +5710,25 @@
         <v>8</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="M4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N4" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="N4" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="O4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="P4" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="Q4" s="20"/>
     </row>
@@ -5825,7 +5788,7 @@
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="8">
         <v>-1</v>
@@ -5933,7 +5896,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="17">
         <v>-1</v>
@@ -6041,7 +6004,7 @@
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B10" s="8">
         <v>-1</v>
@@ -6284,7 +6247,7 @@
         <v>14</v>
       </c>
       <c r="F16" s="4" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>6</v>
@@ -6296,25 +6259,25 @@
         <v>8</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="M16" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N16" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="N16" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="O16" s="4" t="s">
         <v>19</v>
       </c>
       <c r="P16" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="Q16" s="20"/>
     </row>
@@ -6388,7 +6351,7 @@
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A18" s="17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B18" s="17">
         <v>-1</v>
@@ -6524,7 +6487,7 @@
     </row>
     <row r="20" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A20" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B20" s="17">
         <v>-1</v>
@@ -6917,7 +6880,7 @@
         <v>14</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>6</v>
@@ -6929,25 +6892,25 @@
         <v>8</v>
       </c>
       <c r="J28" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="K28" s="4" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="M28" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N28" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="N28" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="O28" s="4" t="s">
         <v>19</v>
       </c>
       <c r="P28" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="Q28" s="20"/>
     </row>
@@ -7021,7 +6984,7 @@
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A30" s="17" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B30" s="17">
         <v>0</v>
@@ -7157,7 +7120,7 @@
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A32" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B32" s="17">
         <v>-1</v>
@@ -7484,7 +7447,7 @@
     </row>
     <row r="39" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A39" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B39" s="6"/>
       <c r="C39" s="16" t="s">
@@ -7550,7 +7513,7 @@
         <v>14</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G40" s="4" t="s">
         <v>6</v>
@@ -7562,25 +7525,25 @@
         <v>8</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="K40" s="4" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="L40" s="4" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="M40" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N40" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="N40" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="O40" s="4" t="s">
         <v>19</v>
       </c>
       <c r="P40" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="Q40" s="20"/>
     </row>
@@ -7654,7 +7617,7 @@
     </row>
     <row r="42" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A42" s="17" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B42" s="17">
         <v>0</v>
@@ -8117,7 +8080,7 @@
     </row>
     <row r="51" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A51" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B51" s="6"/>
       <c r="C51" s="16" t="s">
@@ -8183,7 +8146,7 @@
         <v>14</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G52" s="4" t="s">
         <v>6</v>
@@ -8195,31 +8158,31 @@
         <v>8</v>
       </c>
       <c r="J52" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="K52" s="4" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="L52" s="4" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="M52" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N52" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="N52" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="O52" s="4" t="s">
         <v>19</v>
       </c>
       <c r="P52" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="Q52" s="20"/>
     </row>
     <row r="53" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A53" s="17" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B53" s="17">
         <v>0</v>
@@ -8287,7 +8250,7 @@
     </row>
     <row r="54" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A54" s="17" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B54" s="17">
         <v>0</v>
@@ -8750,7 +8713,7 @@
     </row>
     <row r="63" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B63" s="6"/>
       <c r="C63" s="16" t="s">
@@ -8816,7 +8779,7 @@
         <v>14</v>
       </c>
       <c r="F64" s="4" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G64" s="4" t="s">
         <v>6</v>
@@ -8828,31 +8791,31 @@
         <v>8</v>
       </c>
       <c r="J64" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="K64" s="4" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="L64" s="4" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="M64" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="N64" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="N64" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="O64" s="4" t="s">
         <v>19</v>
       </c>
       <c r="P64" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="Q64" s="22"/>
     </row>
     <row r="65" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A65" s="17" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B65" s="17">
         <v>0</v>
@@ -8917,7 +8880,7 @@
     </row>
     <row r="66" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A66" s="17" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B66" s="17">
         <v>0</v>
@@ -9112,7 +9075,7 @@
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A69" s="17" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B69" s="17">
         <v>0</v>
@@ -9365,7 +9328,7 @@
     </row>
     <row r="75" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A75" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B75" s="6"/>
       <c r="C75" s="16" t="s">
@@ -9423,7 +9386,7 @@
         <v>14</v>
       </c>
       <c r="F76" s="4" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G76" s="4" t="s">
         <v>6</v>
@@ -9435,13 +9398,13 @@
         <v>8</v>
       </c>
       <c r="J76" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="K76" s="4" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="L76" s="4" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="M76" s="4"/>
       <c r="N76" s="4"/>
@@ -9451,7 +9414,7 @@
     </row>
     <row r="77" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A77" s="17" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B77" s="17">
         <v>0</v>
@@ -9497,7 +9460,7 @@
     </row>
     <row r="78" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A78" s="17" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B78" s="17">
         <v>0</v>
@@ -9635,7 +9598,7 @@
     </row>
     <row r="81" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A81" s="17" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B81" s="17">
         <v>900</v>
@@ -9826,7 +9789,7 @@
     </row>
     <row r="87" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A87" s="6" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B87" s="6"/>
       <c r="C87" s="16" t="s">
@@ -9884,7 +9847,7 @@
         <v>14</v>
       </c>
       <c r="F88" s="4" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G88" s="4" t="s">
         <v>6</v>
@@ -9896,13 +9859,13 @@
         <v>8</v>
       </c>
       <c r="J88" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="K88" s="4" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="L88" s="4" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="M88" s="4"/>
       <c r="N88" s="4"/>
@@ -9912,7 +9875,7 @@
     </row>
     <row r="89" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A89" s="17" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B89" s="17">
         <v>0</v>
@@ -9968,7 +9931,7 @@
     </row>
     <row r="90" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A90" s="17" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B90" s="17">
         <v>0</v>
@@ -10080,7 +10043,7 @@
     </row>
     <row r="92" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A92" s="17" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B92" s="17">
         <v>0</v>
@@ -10136,7 +10099,7 @@
     </row>
     <row r="93" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A93" s="17" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B93" s="17">
         <v>900</v>
@@ -10347,7 +10310,7 @@
     </row>
     <row r="99" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A99" s="6" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="B99" s="6"/>
       <c r="C99" s="16" t="s">
@@ -10405,7 +10368,7 @@
         <v>14</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G100" s="4" t="s">
         <v>6</v>
@@ -10417,13 +10380,13 @@
         <v>8</v>
       </c>
       <c r="J100" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="K100" s="4" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="L100" s="4" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="M100" s="4"/>
       <c r="N100" s="4"/>
@@ -10433,7 +10396,7 @@
     </row>
     <row r="101" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A101" s="17" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B101" s="17">
         <v>0</v>
@@ -10489,7 +10452,7 @@
     </row>
     <row r="102" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A102" s="17" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B102" s="17">
         <v>0</v>
@@ -10601,7 +10564,7 @@
     </row>
     <row r="104" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A104" s="17" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B104" s="17">
         <v>0</v>
@@ -10657,7 +10620,7 @@
     </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A105" s="17" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B105" s="17">
         <v>900</v>
@@ -10868,7 +10831,7 @@
     </row>
     <row r="111" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A111" s="6" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
       <c r="B111" s="6"/>
       <c r="C111" s="16" t="s">
@@ -10926,7 +10889,7 @@
         <v>14</v>
       </c>
       <c r="F112" s="4" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="G112" s="4" t="s">
         <v>6</v>
@@ -10938,13 +10901,13 @@
         <v>8</v>
       </c>
       <c r="J112" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="K112" s="4" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="L112" s="4" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="M112" s="4"/>
       <c r="N112" s="4"/>
@@ -10954,7 +10917,7 @@
     </row>
     <row r="113" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A113" s="17" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B113" s="17">
         <v>0</v>
@@ -11113,7 +11076,7 @@
     </row>
     <row r="116" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A116" s="17" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
       <c r="B116" s="17">
         <v>0</v>
@@ -11166,7 +11129,7 @@
     </row>
     <row r="117" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A117" s="17" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B117" s="17">
         <v>900</v>
@@ -11371,20 +11334,20 @@
     </row>
     <row r="121" spans="1:17" x14ac:dyDescent="0.25">
       <c r="G121" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="L121" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="123" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="126" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A126" s="6" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B126" s="6"/>
       <c r="C126" s="16" t="s">
@@ -11429,22 +11392,22 @@
         <v>4</v>
       </c>
       <c r="D127" s="4" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E127" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F127" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G127" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="F127" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G127" s="4" t="s">
-        <v>48</v>
-      </c>
       <c r="H127" s="4" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
       <c r="I127" s="4" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="J127" s="4" t="s">
         <v>6</v>
@@ -11458,7 +11421,7 @@
     </row>
     <row r="128" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A128" s="17" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B128" s="17">
         <v>100000</v>
@@ -11502,7 +11465,7 @@
     </row>
     <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129" s="17" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
       <c r="B129" s="17">
         <v>-20000</v>
@@ -11635,22 +11598,22 @@
     </row>
     <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D132" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E132" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F132" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G132" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="H132" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="I132" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="J132" t="s">
         <v>13</v>
@@ -11659,7 +11622,7 @@
         <v>14</v>
       </c>
       <c r="L132" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -11699,6 +11662,10 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" scale="60" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;18Ejercicio 10</oddHeader>
+  </headerFooter>
 </worksheet>
 </file>
 
@@ -11706,8 +11673,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9F485CE0-8B47-41FB-BCFC-81CEA9BA3E4B}">
   <dimension ref="A3:N92"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="I95" sqref="I95"/>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11780,25 +11747,25 @@
         <v>8</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="J4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K4" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="K4" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="L4" s="4" t="s">
         <v>19</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="N4" s="20"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" s="8">
         <v>-1</v>
@@ -11843,7 +11810,7 @@
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" s="8">
         <v>-1</v>
@@ -11933,7 +11900,7 @@
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B8" s="8">
         <v>-1</v>
@@ -12143,19 +12110,19 @@
         <v>8</v>
       </c>
       <c r="I14" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="J14" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K14" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="K14" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="L14" s="4" t="s">
         <v>19</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="N14" s="20"/>
     </row>
@@ -12217,7 +12184,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="12">
         <v>-1</v>
@@ -12329,7 +12296,7 @@
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B18" s="12">
         <v>-1</v>
@@ -12550,19 +12517,19 @@
         <v>8</v>
       </c>
       <c r="I24" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="J24" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K24" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="L24" s="4" t="s">
         <v>19</v>
       </c>
       <c r="M24" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="N24" s="20"/>
     </row>
@@ -12624,7 +12591,7 @@
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B26" s="12">
         <v>-1</v>
@@ -12891,7 +12858,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B33" s="6"/>
       <c r="C33" s="13" t="s">
@@ -12957,19 +12924,19 @@
         <v>8</v>
       </c>
       <c r="I34" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="J34" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K34" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="K34" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="L34" s="4" t="s">
         <v>19</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="N34" s="20"/>
     </row>
@@ -13031,7 +12998,7 @@
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B36" s="12">
         <v>-1</v>
@@ -13087,7 +13054,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="12" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B37" s="12">
         <v>0</v>
@@ -13298,7 +13265,7 @@
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B43" s="6"/>
       <c r="C43" s="13" t="s">
@@ -13364,19 +13331,19 @@
         <v>8</v>
       </c>
       <c r="I44" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="J44" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K44" s="4" t="s">
         <v>22</v>
-      </c>
-      <c r="K44" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="L44" s="4" t="s">
         <v>19</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="N44" s="20"/>
     </row>
@@ -13488,7 +13455,7 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="12" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B47" s="12">
         <v>0</v>
@@ -13693,7 +13660,7 @@
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B53" s="6"/>
       <c r="C53" s="13" t="s">
@@ -13751,7 +13718,7 @@
         <v>8</v>
       </c>
       <c r="I54" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="J54" s="4"/>
       <c r="K54" s="4"/>
@@ -13835,7 +13802,7 @@
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="12" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="B57" s="12">
         <v>0</v>
@@ -13984,7 +13951,7 @@
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B63" s="6"/>
       <c r="C63" s="13" t="s">
@@ -14042,7 +14009,7 @@
         <v>8</v>
       </c>
       <c r="I64" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="J64" s="4"/>
       <c r="K64" s="4"/>
@@ -14303,7 +14270,7 @@
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B73" s="6"/>
       <c r="C73" s="13" t="s">
@@ -14361,7 +14328,7 @@
         <v>8</v>
       </c>
       <c r="I74" s="4" t="s">
-        <v>50</v>
+        <v>43</v>
       </c>
       <c r="J74" s="4"/>
       <c r="K74" s="4"/>
@@ -14610,20 +14577,20 @@
     </row>
     <row r="81" spans="1:10" x14ac:dyDescent="0.25">
       <c r="F81" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="I81" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="83" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="86" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A86" s="6" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="B86" s="6"/>
       <c r="C86" s="14" t="s">
@@ -14662,16 +14629,16 @@
         <v>4</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="E87" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F87" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G87" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="F87" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G87" s="4" t="s">
-        <v>48</v>
       </c>
       <c r="H87" s="4" t="s">
         <v>6</v>
@@ -14683,7 +14650,7 @@
     </row>
     <row r="88" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A88" s="15" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="B88" s="15">
         <v>0.4</v>
@@ -14717,7 +14684,7 @@
     </row>
     <row r="89" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A89" s="15" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B89" s="15">
         <v>1.7</v>
@@ -14785,7 +14752,7 @@
     </row>
     <row r="91" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A91" s="18" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B91" s="18"/>
       <c r="C91" s="18"/>
@@ -14816,16 +14783,16 @@
     </row>
     <row r="92" spans="1:10" x14ac:dyDescent="0.25">
       <c r="D92" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="H92" s="1" t="s">
         <v>13</v>
@@ -14866,6 +14833,10 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>
+  <headerFooter>
+    <oddHeader>&amp;C&amp;18Ejercicio 11 y 12</oddHeader>
+  </headerFooter>
   <ignoredErrors>
     <ignoredError sqref="C37 D37:M37" formula="1"/>
   </ignoredErrors>

</xml_diff>